<commit_message>
RmD andf SoE Updates
Inline coding in R markdown fixed, summary of evidence tables edited.
</commit_message>
<xml_diff>
--- a/data/human/LSR1_H_SOE.xlsx
+++ b/data/human/LSR1_H_SOE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkennett\Documents\GitHub\LSR1_anhedonia_H\data\human\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4D589D-11CA-4703-9A9B-E1691FEA90E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C21E9D3-5B27-4A69-BCFF-63D9A36D35D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7270" xr2:uid="{09461E91-9619-4CA9-A1C2-25F30588097D}"/>
+    <workbookView xWindow="29985" yWindow="585" windowWidth="26625" windowHeight="14820" xr2:uid="{09461E91-9619-4CA9-A1C2-25F30588097D}"/>
   </bookViews>
   <sheets>
     <sheet name="SOE" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
   <si>
     <t>Pro-dopaminergic intervention. vs placebo in depressed patients with symptoms of anhedonia  </t>
   </si>
@@ -699,13 +699,22 @@
       </rPr>
       <t>t2=0</t>
     </r>
+  </si>
+  <si>
+    <t>Timepoint</t>
+  </si>
+  <si>
+    <t>8 weeks</t>
+  </si>
+  <si>
+    <t>4-12 weeks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -743,6 +752,12 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1306,245 +1321,275 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C433B388-4C10-4695-879F-238B8D5178E7}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.90625" customWidth="1"/>
-    <col min="2" max="2" width="20.36328125" customWidth="1"/>
-    <col min="3" max="3" width="14.90625" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" customWidth="1"/>
-    <col min="6" max="6" width="11.26953125" customWidth="1"/>
+    <col min="1" max="2" width="16.90625" customWidth="1"/>
+    <col min="3" max="3" width="20.36328125" customWidth="1"/>
+    <col min="4" max="4" width="24.453125" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="25.453125" customWidth="1"/>
+    <col min="7" max="7" width="23.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="67.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
-    <row r="2" spans="1:7" ht="405" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="189" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:7" ht="175.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="108" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="148.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="94.5" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="132.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="132.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="D5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="F5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="G5" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="132.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="132.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="G6" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="133.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="G7" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="137.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" ht="137.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="F8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="G8" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="131.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" ht="131.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="G9" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="162.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" ht="81.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="G10" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="175.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="94.5" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="D11" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="E11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="F11" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="G11" s="16" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Change to analysis script, TOC, SoE, RoB-ME
dfamendments script altered, analysis re-run and checked, ToC altered, SoE finalised, RoB-ME matrix added.
</commit_message>
<xml_diff>
--- a/data/human/LSR1_H_SOE.xlsx
+++ b/data/human/LSR1_H_SOE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkennett\Documents\GitHub\LSR1_anhedonia_H\data\human\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C21E9D3-5B27-4A69-BCFF-63D9A36D35D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0F2F2C-A42E-4827-8F61-E774A0250C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29985" yWindow="585" windowWidth="26625" windowHeight="14820" xr2:uid="{09461E91-9619-4CA9-A1C2-25F30588097D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{09461E91-9619-4CA9-A1C2-25F30588097D}"/>
   </bookViews>
   <sheets>
     <sheet name="SOE" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
   <si>
     <t>Pro-dopaminergic intervention. vs placebo in depressed patients with symptoms of anhedonia  </t>
   </si>
@@ -181,9 +181,6 @@
     <t>Acceptability of pro-dopaminergic interventions vs placebo </t>
   </si>
   <si>
-    <t>Low risk: 10% of studies had an overall high risk of bias, primarily due to concerns over outcome measurement, while 32% were rated moderate risk of bias. </t>
-  </si>
-  <si>
     <t>Low risk: the impact of bias on the magnitude and direction of the effects of pro-dopaminergic agonists is low. </t>
   </si>
   <si>
@@ -293,27 +290,92 @@
     <t>Moderate risk: 33% of the studies had an overall high risk of bias (due to missing outcome data, and issues with outcome measurement and selective reporting of findings. 33% of studies had a moderate risk of bias.) </t>
   </si>
   <si>
-    <r>
-      <t>N=50, n=9168; Random effects: OR=0.96, 95%CI: 0.78,  1.18, I</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">=62% </t>
+    <t>Low risk: 59% of studies were rated low risk of bias and only 8% were rated high risk of bias. </t>
+  </si>
+  <si>
+    <t>Moderate risk: 83% of studies were rated at least some concerns in RoB2 domain 5, selection of results. The impact of the bias on the magnitude and direction of the effects of pro-dopaminergic agonists is unclear. </t>
+  </si>
+  <si>
+    <t>Moderate risk: 83% of the studies measured the same intervention, bupropion.For outcomes, 50% of studies measured anhedonia using the MEI, 33% using the MADRS anhedonia item and 17% using the IDS-IVR-30/IDS-C-30 Pleasure Scale  No other clear indication of indirectness in terms of population, interventions, and outcomes.  </t>
+  </si>
+  <si>
+    <t>Moderate risk: 73% of studies were rated moderate risk of bias while 18% were rated as high risk of bias. This was primarily due to domain 2- deviation from intended interventions. </t>
+  </si>
+  <si>
+    <t>Moderate risk: 55% of studies were rated moderate risk in domain 5 of RoB2. The impact of the bias on the magnitude and direction of the effects is unclear. </t>
+  </si>
+  <si>
+    <t>Moderate risk: 73% of studies contributing to the analysis tested bupropion  </t>
+  </si>
+  <si>
+    <t>Low risk: 67% of studies were rated low risk of bias for RoB2 while only 4% were rated high risk of bias. </t>
+  </si>
+  <si>
+    <t>Low risk: 65% of studies were rated low risk for RoB2 while 31% were rated as moderate risk with scores of ‘some concerns’ spread out across domains in no clear pattern. </t>
+  </si>
+  <si>
+    <r>
+      <t>N=5, n=962, random effects OR=1.90, 95%CI: 0.90, 4.00, I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">=2% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>t2=0</t>
+    </r>
+  </si>
+  <si>
+    <t>Timepoint</t>
+  </si>
+  <si>
+    <t>8 weeks</t>
+  </si>
+  <si>
+    <t>4-12 weeks</t>
+  </si>
+  <si>
+    <r>
+      <t>N=52, n=9725; Random effects: OR=0.97, 95%CI: 0.79,  1.17, I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">=61% </t>
     </r>
     <r>
       <rPr>
@@ -338,12 +400,64 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>=0.240 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>N=19, n=4818; random effects: OR=1.55, 95%CI: 1.25, 1.93, I</t>
+      <t>=0.222 </t>
+    </r>
+  </si>
+  <si>
+    <t>Tolerability of pro-dopaminergic interventions vs placebo </t>
+  </si>
+  <si>
+    <r>
+      <t>N=43, n=9030; Random effects: OR=1.83, 95%CI: 1.38,  2.41, I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">=35% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>=0.223 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>N=21, n=5375; random effects: OR=1.46, 95%CI: 1.17, 1.82, I</t>
     </r>
     <r>
       <rPr>
@@ -392,7 +506,7 @@
   </si>
   <si>
     <r>
-      <t>N=22, n=5469, random effects OR=1.72, 95%CI: 1.32, 2.23, I</t>
+      <t>N=24, n=6026, random effects OR=1.70, 95%CI: 1.32, 2.18, I</t>
     </r>
     <r>
       <rPr>
@@ -436,52 +550,31 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>=0.080 </t>
-    </r>
-  </si>
-  <si>
-    <t>Low risk: 59% of studies were rated low risk of bias and only 8% were rated high risk of bias. </t>
-  </si>
-  <si>
-    <t>Moderate risk: 83% of studies were rated at least some concerns in RoB2 domain 5, selection of results. The impact of the bias on the magnitude and direction of the effects of pro-dopaminergic agonists is unclear. </t>
-  </si>
-  <si>
-    <t>Moderate risk: 83% of the studies measured the same intervention, bupropion.For outcomes, 50% of studies measured anhedonia using the MEI, 33% using the MADRS anhedonia item and 17% using the IDS-IVR-30/IDS-C-30 Pleasure Scale  No other clear indication of indirectness in terms of population, interventions, and outcomes.  </t>
-  </si>
-  <si>
-    <t>Moderate risk: 73% of studies were rated moderate risk of bias while 18% were rated as high risk of bias. This was primarily due to domain 2- deviation from intended interventions. </t>
-  </si>
-  <si>
-    <t>Moderate risk: 55% of studies were rated moderate risk in domain 5 of RoB2. The impact of the bias on the magnitude and direction of the effects is unclear. </t>
-  </si>
-  <si>
-    <t>Moderate risk: 73% of studies contributing to the analysis tested bupropion  </t>
-  </si>
-  <si>
-    <t>Low risk: 74% of studies were rated as low risk of bias and 5% were rated high risk of bias. </t>
-  </si>
-  <si>
-    <r>
-      <t>N=24, n=6308, random effects OR=2.12, 95%CI: 1.68, 2.67, I</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">=36% </t>
+      <t>=0.083 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>N=26, n=6865, random effects OR=2.13, 95%CI: 1.73, 2.63, I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">=32% </t>
     </r>
     <r>
       <rPr>
@@ -506,12 +599,12 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>=0.080</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>N=26, n=6527, random effects, OR=1.16, 95%CI: 1.03, 1.31, I</t>
+      <t>=0.053</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>N=28, n=7084, random effects, OR=1.14, 95%CI: 1.02, 1.28, I</t>
     </r>
     <r>
       <rPr>
@@ -559,33 +652,27 @@
     </r>
   </si>
   <si>
-    <t>Low risk: 67% of studies were rated low risk of bias for RoB2 while only 4% were rated high risk of bias. </t>
-  </si>
-  <si>
-    <t>Low risk: 65% of studies were rated low risk for RoB2 while 31% were rated as moderate risk with scores of ‘some concerns’ spread out across domains in no clear pattern. </t>
-  </si>
-  <si>
-    <r>
-      <t>N=24, n=6489, random effects OR=1.46, 95%CI: 1.18, 1.79, I</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">=27% </t>
+    <r>
+      <t>N=26, n=6489, random effects OR=1.46, 95%CI: 1.21, 1.76, I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">=22% </t>
     </r>
     <r>
       <rPr>
@@ -610,34 +697,31 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>=0.064 </t>
-    </r>
-  </si>
-  <si>
-    <t>Low risk: 67% of studies were rated low risk for RoB2 while 21% were rated moderate. </t>
-  </si>
-  <si>
-    <r>
-      <t>N=22, n=5875, random effects OR=1.79, 95%CI: 1.42, 2.25, I</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">=5% </t>
+      <t>=0.043 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>N=24, n=6432, random effects OR=1.81, 95%CI: 1.46, 2.25, I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">=7% </t>
     </r>
     <r>
       <rPr>
@@ -662,52 +746,23 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>=0.030 </t>
-    </r>
-  </si>
-  <si>
-    <t>Low risk: 64% of studies were rated as low risk for RoB2 while 32% were rated as moderate risk. </t>
-  </si>
-  <si>
-    <r>
-      <t>N=5, n=962, random effects OR=1.90, 95%CI: 0.90, 4.00, I</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">=2% </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>t2=0</t>
-    </r>
-  </si>
-  <si>
-    <t>Timepoint</t>
-  </si>
-  <si>
-    <t>8 weeks</t>
-  </si>
-  <si>
-    <t>4-12 weeks</t>
+      <t>=0.031 </t>
+    </r>
+  </si>
+  <si>
+    <t>Low risk: 10% of studies had an overall high risk of bias, primarily due to concerns over outcome measurement, while 31% were rated moderate risk of bias. </t>
+  </si>
+  <si>
+    <t>Low risk: 12% of studies had an overall high risk of bias, primarily due to concerns over outcome measurement, while 35% were rated moderate risk of bias. </t>
+  </si>
+  <si>
+    <t>Low risk: 77% of studies were rated as low risk of bias and 5% were rated high risk of bias. </t>
+  </si>
+  <si>
+    <t>Low risk: 73% of studies were rated low risk for RoB2 while 23% were rated moderate. </t>
+  </si>
+  <si>
+    <t>Low risk: 68% of studies were rated as low risk for RoB2 while 28% were rated as moderate risk. </t>
   </si>
 </sst>
 </file>
@@ -1321,10 +1376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C433B388-4C10-4695-879F-238B8D5178E7}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1342,7 +1397,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>3</v>
@@ -1366,19 +1421,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="E2" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>1</v>
@@ -1390,19 +1445,19 @@
         <v>8</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>1</v>
@@ -1413,178 +1468,205 @@
         <v>10</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="132.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="10" t="s">
+    <row r="5" spans="1:8" ht="94.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="C5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>16</v>
+      <c r="G5" s="8" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="132.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="132.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="133.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="B8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="7" spans="1:8" ht="133.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="12" t="s">
+    <row r="9" spans="1:8" ht="137.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="5" t="s">
+      <c r="B9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="13" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="8" spans="1:8" ht="137.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="9" t="s">
+    <row r="10" spans="1:8" ht="131.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="10" t="s">
+      <c r="B10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="9" spans="1:8" ht="131.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="5" t="s">
+    <row r="11" spans="1:8" ht="81.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>16</v>
+      <c r="B11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="81.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="5" t="s">
+    <row r="12" spans="1:8" ht="108" x14ac:dyDescent="0.35">
+      <c r="A12" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="94.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="14" t="s">
+      <c r="B12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="15" t="s">
+      <c r="E12" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="F12" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="16" t="s">
+      <c r="G12" s="16" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>